<commit_message>
The Project has been completed
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/inputdata.xlsx
+++ b/src/test/resources/testdata/inputdata.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Manali</t>
   </si>
@@ -36,13 +36,226 @@
   </si>
   <si>
     <t>Bengaluru</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>adults</t>
+  </si>
+  <si>
+    <t>children</t>
+  </si>
+  <si>
+    <t>infants</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <r>
+      <t>Mobile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>no</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Mobile</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>No</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>message</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>travel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Please</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>enter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>valid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFCCCCCC"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>number</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,8 +265,32 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF008000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,9 +313,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,28 +602,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="3"/>
+    <col min="3" max="3" width="13.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="3" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="3"/>
+    <col min="9" max="9" width="11" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="15.109375" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8438542755</v>
+      </c>
+      <c r="D2" s="4">
+        <v>12345</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>